<commit_message>
API TCs and Bugs
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Mr-Mandoob\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0289FA1-6E21-4EDE-9F3A-D70B4E9B5605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B71DB9C-34B4-464C-B1AD-209390CC38CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>Bug ID</t>
   </si>
@@ -67,13 +67,106 @@
   </si>
   <si>
     <t>b6</t>
+  </si>
+  <si>
+    <t>Check the attached file called b1</t>
+  </si>
+  <si>
+    <t>Check the attached file called b2</t>
+  </si>
+  <si>
+    <t>Check the attached file called b3</t>
+  </si>
+  <si>
+    <t>Check the attached file called b4</t>
+  </si>
+  <si>
+    <t>Check the attached file called b5</t>
+  </si>
+  <si>
+    <t>Check the attached file called b6</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy j4 with Android 9</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> App works correctly in cases (receiving a phone call, SMS, low battery, high screen brightness, and low screen brightness)</t>
+  </si>
+  <si>
+    <t>WIFI</t>
+  </si>
+  <si>
+    <t>App crashes when opening the notifications from mobile notifications bar while App not opened</t>
+  </si>
+  <si>
+    <t>in Your teams tab Add your team button disappear in portrait mode</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Any team name which contains two words in vertical mode the second word is missing</t>
+  </si>
+  <si>
+    <t>1- Launch Yallakora App.                        2- Click matches tab.                                      3- Scroll down to the European matches.                                                    4- Click north irland match.             Word north is missing and when clicking on the match finished lab not fully appeared and there is no data in formation.</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Download Yallakora for Play store.                                                        2- Launch the App then close it wait a while you will receive notifications in the phone notifications bar.                                    3- Click the received notification. I didn't open.                                                    </t>
+  </si>
+  <si>
+    <t>1- Launch Yallakora App.                        2- Click your teams tab.                     3- Change your phone to Portrait mode.                                                       Add your team button disappeared.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Launch Yallakora App.                        2- Click matches tab.                             3- Select Tuesday 14 June, First finished match between cheli and Gana there is two results (0-0 and 3-1)    </t>
+  </si>
+  <si>
+    <t>There is two results for a finished match between Cheli and Gana</t>
+  </si>
+  <si>
+    <t>Medium as when you click the match it shows the right result</t>
+  </si>
+  <si>
+    <t>High as this is a kora App news</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Launch Yallakora App.                        2- Click Your teams tab.                     Also I didn't add teams but the upper right side update sign is active.  </t>
+  </si>
+  <si>
+    <t>The update teams sign is active also I didn't add teams yet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low as when click the update sign it opens to selcet team </t>
+  </si>
+  <si>
+    <t>Low as the update sign color the same if it active or inactive</t>
+  </si>
+  <si>
+    <t>There is invalid date word for first item of important news in home (as it an Ad not a news) and sharing it  take about two seconds to open sharing options</t>
+  </si>
+  <si>
+    <t>1- Launch Yallakora App.                        2- Click Home tab.                                3- Scroll down to Important news check first item (An Ad)it's has invaild date and when clicking it and click the upper right side sharing sign it takes about two seconds (this more than usual )to open sharing options.</t>
+  </si>
+  <si>
+    <t>Critical as this is the Home tab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +188,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -138,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -150,6 +251,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +547,7 @@
     <col min="4" max="4" width="30.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -471,77 +576,161 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -573,15 +762,13 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -603,6 +790,26 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>